<commit_message>
Roles y Responsabilidades - Actualizacion Matriz
</commit_message>
<xml_diff>
--- a/Entregables/Roles y Responsabilidades/Matriz Roles y responsabilidades.xlsx
+++ b/Entregables/Roles y Responsabilidades/Matriz Roles y responsabilidades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="41">
   <si>
     <t>PM</t>
   </si>
@@ -56,9 +56,6 @@
     <t>E</t>
   </si>
   <si>
-    <t>P/I</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Gantt</t>
   </si>
   <si>
-    <t>E/C</t>
-  </si>
-  <si>
     <t>Documento de arquitectura</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>Poster</t>
   </si>
   <si>
-    <t>I/P</t>
-  </si>
-  <si>
     <t>Estudio de factibilidad</t>
   </si>
   <si>
@@ -152,10 +143,10 @@
     <t>Plan de pruebas</t>
   </si>
   <si>
-    <t>Columna1</t>
-  </si>
-  <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Entregable</t>
   </si>
 </sst>
 </file>
@@ -303,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -321,9 +312,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -711,8 +699,11 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:I30" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="11" tableBorderDxfId="12">
   <autoFilter ref="A1:I30"/>
+  <sortState ref="A2:I30">
+    <sortCondition ref="A1:A30"/>
+  </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="Columna1" dataDxfId="10"/>
+    <tableColumn id="1" name="Entregable" dataDxfId="10"/>
     <tableColumn id="2" name="PM" dataDxfId="9"/>
     <tableColumn id="3" name="AF" dataDxfId="8"/>
     <tableColumn id="4" name="DBA" dataDxfId="7"/>
@@ -992,41 +983,41 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1038,700 +1029,700 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="H14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="8"/>
-    </row>
-    <row r="17" spans="1:9" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D17" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="8"/>
-    </row>
-    <row r="18" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="C18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="B23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="8"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="B24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="8"/>
-    </row>
-    <row r="25" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="8"/>
-    </row>
-    <row r="26" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I26" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>39</v>
+        <v>10</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" s="8"/>
-    </row>
-    <row r="30" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I30" s="14"/>
+        <v>12</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>